<commit_message>
Added some files updated last protocol + journal
</commit_message>
<xml_diff>
--- a/documents/03_QM/FRVA_Arbeitsjournal.xlsx
+++ b/documents/03_QM/FRVA_Arbeitsjournal.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitslog" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Pivot Table_Arbeitslog_1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Pivot Table_Arbeitslog" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="WBS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t xml:space="preserve">Wer</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t xml:space="preserve">Patrick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kick-Off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Besprechung weiteres Vorgehen</t>
   </si>
   <si>
     <t xml:space="preserve">Sum - Wie lange</t>
@@ -199,7 +205,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="17">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -230,6 +236,13 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right style="medium"/>
       <top style="medium"/>
       <bottom style="thin"/>
@@ -257,6 +270,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="medium"/>
       <top style="thin"/>
@@ -264,58 +284,16 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -335,7 +313,7 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
-      <right style="thin"/>
+      <right/>
       <top style="thin"/>
       <bottom style="medium"/>
       <diagonal/>
@@ -391,7 +369,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -404,6 +382,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -420,7 +402,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -428,39 +410,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="8" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -468,27 +462,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -511,35 +485,45 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="2">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="6">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:E3" sheet="Arbeitslog"/>
+    <worksheetSource ref="A1:E500" sheet="Arbeitslog"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Wer" numFmtId="0">
-      <sharedItems count="2" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+      <sharedItems count="3" containsMixedTypes="1" containsSemiMixedTypes="1" containsString="1" containsNumber="0">
         <s v="Patrick"/>
         <s v="Roland"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Wann" numFmtId="0">
-      <sharedItems count="1" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
+      <sharedItems count="3" containsMixedTypes="1" containsSemiMixedTypes="1" containsString="0" containsNumber="1">
         <n v="42957"/>
+        <n v="42971"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Wie lange" numFmtId="0">
-      <sharedItems count="1" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
+      <sharedItems count="4" containsMixedTypes="1" containsSemiMixedTypes="1" containsString="0" containsNumber="1">
+        <n v="1"/>
+        <n v="3"/>
         <n v="5"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Arbeitspacket (WBS)" numFmtId="0">
-      <sharedItems count="1" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+      <sharedItems count="2" containsMixedTypes="1" containsSemiMixedTypes="1" containsString="1" containsNumber="0">
         <s v="1.01 Meetings"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Was" numFmtId="0">
-      <sharedItems count="1" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+      <sharedItems count="4" containsMixedTypes="1" containsSemiMixedTypes="1" containsString="1" containsNumber="0">
+        <s v="Besprechung weiteres Vorgehen"/>
+        <s v="Kick-Off"/>
         <s v="Planung Kick-Off, Projektstart, vorbereitung Dokumentation"/>
+        <m/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -547,17 +531,45 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="2">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="6">
   <r>
     <x v="1"/>
     <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
@@ -567,7 +579,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
-  <location ref="A1:D7" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
+  <location ref="A1:E5" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0"/>
     <pivotField axis="axisCol" showAll="0"/>
@@ -579,9 +591,8 @@
     <field x="0"/>
     <field x="3"/>
   </rowFields>
-  <colFields count="2">
+  <colFields count="1">
     <field x="1"/>
-    <field x="-2"/>
   </colFields>
   <dataFields count="1">
     <dataField fld="2" subtotal="sum"/>
@@ -594,19 +605,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="51.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.83"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,7 +647,7 @@
       <c r="C2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -653,23 +664,91 @@
       <c r="C3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>42971</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>42971</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>42971</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>42971</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D3" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D7" type="list">
       <formula1>WBS!$A$1:$E$43</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -682,101 +761,100 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.83"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="11" t="n">
+        <v>42957</v>
+      </c>
+      <c r="D2" s="12" t="n">
+        <v>42971</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" s="18" t="n">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="9" t="n">
-        <v>42957</v>
-      </c>
-      <c r="D2" s="10" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="18" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="D5" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" s="18" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="20" t="n">
-        <v>5</v>
-      </c>
-      <c r="D6" s="18" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="D7" s="24" t="n">
-        <v>10</v>
+      <c r="E5" s="23" t="n">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -791,35 +869,35 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.5612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,114 +905,114 @@
         <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>